<commit_message>
inititialisation capture mobile et teste mobile
</commit_message>
<xml_diff>
--- a/testes.xlsx
+++ b/testes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\m2\14_tpt\livrable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB13014A-31CF-4838-B612-831543401CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10918213-B79C-4F15-8768-B94610F255A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{7F025D69-804F-465E-94E1-9F1C08CF96A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{7F025D69-804F-465E-94E1-9F1C08CF96A4}"/>
   </bookViews>
   <sheets>
     <sheet name="bureau" sheetId="1" r:id="rId1"/>
+    <sheet name="mobile" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>Auteur</t>
   </si>
@@ -180,6 +181,60 @@
 date début: 2023-09-09
 date fin: 2021-09-10
 confirmer</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>Démarrage de l'app</t>
+  </si>
+  <si>
+    <t>cliquer l'icon</t>
+  </si>
+  <si>
+    <t>splash screen
+apparition du login</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>conditions generales</t>
+  </si>
+  <si>
+    <t>cliquer le bouton conditions generlaes</t>
+  </si>
+  <si>
+    <t>chargement
+apparition des conditions generales</t>
+  </si>
+  <si>
+    <t>multi-lingue</t>
+  </si>
+  <si>
+    <t>cliquer l'icon retour
+choisir la langue malgache
+cliquer le bouton conditions generlaes</t>
+  </si>
+  <si>
+    <t>l'app est en malgache
+chargement
+apparition des conditions generales en malgaches</t>
+  </si>
+  <si>
+    <t>remplir le formulaire par
+email: teste@gmail.com
+mots de passe: testestes</t>
+  </si>
+  <si>
+    <t>inscription</t>
+  </si>
+  <si>
+    <t>cliquer creer un compte
+remplir le formulaire par
+nom complet: 
+email: teste@gmail.com
+mots de passe: testestes</t>
   </si>
 </sst>
 </file>
@@ -203,12 +258,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -223,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -233,6 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8AE7661-560E-4E91-AFD5-AF1F9BA30C04}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,4 +841,120 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A128FEB8-44D3-4E60-8D40-9B87BB3C77B2}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.140625" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" customWidth="1"/>
+    <col min="3" max="3" width="52.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
retest final back office
</commit_message>
<xml_diff>
--- a/testes.xlsx
+++ b/testes.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\m2\14_tpt\livrable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\M2\tpt-2021\master\mbdsp7TanjonaOliviaAnah\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10918213-B79C-4F15-8768-B94610F255A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{7F025D69-804F-465E-94E1-9F1C08CF96A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="bureau" sheetId="1" r:id="rId1"/>
     <sheet name="mobile" sheetId="2" r:id="rId2"/>
+    <sheet name="Back Office" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="120">
   <si>
     <t>Auteur</t>
   </si>
@@ -236,11 +236,195 @@
 email: teste@gmail.com
 mots de passe: testestes</t>
   </si>
+  <si>
+    <t>Test case</t>
+  </si>
+  <si>
+    <t>Back office</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auteur </t>
+  </si>
+  <si>
+    <t>Tanjona</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>login avec email admin@admin.com mot de passe : 12345678</t>
+  </si>
+  <si>
+    <t>login avec email admin@admin.com mot de passe : azetf</t>
+  </si>
+  <si>
+    <t>Reste sur le page login avec notification : Email ou mot de passe invalide</t>
+  </si>
+  <si>
+    <t>reste sur le page login avec notification : Email invalid et mot de passe superieur à 8 caractère</t>
+  </si>
+  <si>
+    <t xml:space="preserve">login avec email admin@ad et mot de passe : azert </t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>Clique sur l'image du profile en haute droite et puis Profil</t>
+  </si>
+  <si>
+    <t>Page profile avec les informations</t>
+  </si>
+  <si>
+    <t>Modification information : nom complet : Admin en Administrateur, changer image en fichier .txt</t>
+  </si>
+  <si>
+    <t>Reste sur le page profile avec notification : Error: Fichier autorisé : .png, .jpg et .jpeg !</t>
+  </si>
+  <si>
+    <t>Modification information : nom complet : Admin en Administrateur, changer image en fichier .jpg</t>
+  </si>
+  <si>
+    <t>Modification information avec notification : Modification réussi !</t>
+  </si>
+  <si>
+    <t>Changement mot de passe : clique sur le bouton : Changer mot de passe</t>
+  </si>
+  <si>
+    <t>Page profile avec formulaire de changement mot de passe</t>
+  </si>
+  <si>
+    <t>remplir le formulaire avec mot de passe actuel : 12345678 et nouveau mot de passe : 1234azert!</t>
+  </si>
+  <si>
+    <t>page profile avec formulaire de changement mot de passe et notification : Changement mot de passe réussi !</t>
+  </si>
+  <si>
+    <t>Gestion  utilisateur</t>
+  </si>
+  <si>
+    <t>Clique sur le navigation : Gestion utilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liste des utilisateurs avec ses commentaire faites </t>
+  </si>
+  <si>
+    <t>Bloquer utilisateur qui a des commentaires signalés  en cliquant sur le bouton Bloquer activer</t>
+  </si>
+  <si>
+    <t>Message de confirmation de blocage: Si oui l'utilisateur est bloqué en commentaire et l'action devient débloquer</t>
+  </si>
+  <si>
+    <t>Debloquer  utilisateur</t>
+  </si>
+  <si>
+    <t>Message de confirmation de blocage: Si oui l'utilisateur est débloqué en commentaire et l'action devient bloquer</t>
+  </si>
+  <si>
+    <t>Gestion modérateur ajout</t>
+  </si>
+  <si>
+    <t>Page d'inscription modérateur</t>
+  </si>
+  <si>
+    <t>remplir le formulaire avec les informations validés : nom : moderateur1 , email:moderateur@gmail.com, datenaissance : 24/02/1998, mot de passe : 12345678, image profile</t>
+  </si>
+  <si>
+    <t>page d'inscription avec formulaire vide et notification : Ajout modérateur réussi !</t>
+  </si>
+  <si>
+    <t>Gestion modérateur Liste</t>
+  </si>
+  <si>
+    <t>liste paginé des moderateurs créées</t>
+  </si>
+  <si>
+    <t>Modification moderateur en cliquant sur le l'icon modifier</t>
+  </si>
+  <si>
+    <t>page de modification moderateur</t>
+  </si>
+  <si>
+    <t>Clique sur le navigation : Modérateur et ajout</t>
+  </si>
+  <si>
+    <t>Clique sur le navigation : Modérateur et liste</t>
+  </si>
+  <si>
+    <t>Modification  email en mod@gmail.com et date Naissance en 02/03/1998</t>
+  </si>
+  <si>
+    <t>Suppression moderateur</t>
+  </si>
+  <si>
+    <t>Message de confirmation : si non : rien, et si oui : suppression de moderateur de la liste</t>
+  </si>
+  <si>
+    <t>Deconnexion</t>
+  </si>
+  <si>
+    <t>Clique sur l'image en haut droite et deconnexion</t>
+  </si>
+  <si>
+    <t>page login</t>
+  </si>
+  <si>
+    <t>Reconnexion admin en nouveau mot de passe</t>
+  </si>
+  <si>
+    <t>login avec email admin@admin.com mot de passe : 1234azert!</t>
+  </si>
+  <si>
+    <t>Page d'accueil</t>
+  </si>
+  <si>
+    <t>Mot de passe oublié</t>
+  </si>
+  <si>
+    <t>En cliquant sur le lien Mot de passe oublié! du page login</t>
+  </si>
+  <si>
+    <t>Page verification mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remplir le formulaire avec email </t>
+  </si>
+  <si>
+    <t>Si email touvé : page de nouveau mot de passe .si non : reste sur la avec notification : Email introuvable</t>
+  </si>
+  <si>
+    <t>changer mot de passe avec : 987654321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notification : Changement mot de passe réussi !
+</t>
+  </si>
+  <si>
+    <t>Login moderateur</t>
+  </si>
+  <si>
+    <t>login avec email : mod@gmail.com et mot de passe: 987654321</t>
+  </si>
+  <si>
+    <t>Page accueil avec navigation : Gestion utilisateur</t>
+  </si>
+  <si>
+    <t>Page accueil : dashboard , Navigation : Gestion utilisateur, Moderateur avec Token de 300 secondes</t>
+  </si>
+  <si>
+    <t>Dashbord</t>
+  </si>
+  <si>
+    <t>en cliquant sur le navigation : Dashbord</t>
+  </si>
+  <si>
+    <t>Page dashboard avec : recharge total faites par les clients, nombre de client,nombre de match,statistique recharge par mois, progression match</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -284,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -295,6 +479,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,14 +804,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8AE7661-560E-4E91-AFD5-AF1F9BA30C04}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.42578125" customWidth="1"/>
     <col min="2" max="2" width="44.5703125" customWidth="1"/>
@@ -844,14 +1040,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A128FEB8-44D3-4E60-8D40-9B87BB3C77B2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.140625" customWidth="1"/>
     <col min="2" max="2" width="51.85546875" customWidth="1"/>
@@ -879,7 +1075,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -957,4 +1153,354 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="56" customWidth="1"/>
+    <col min="3" max="3" width="42.85546875" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ipa, exe, teste finale
</commit_message>
<xml_diff>
--- a/testes.xlsx
+++ b/testes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\m2\14_tpt\livrable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320AFE1B-F6EE-47CA-8D36-610A44A555D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367896FF-6402-4194-A696-FDC9C1DB962D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bureau" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="168">
   <si>
     <t>Auteur</t>
   </si>
@@ -231,13 +231,6 @@
     <t>inscription</t>
   </si>
   <si>
-    <t>cliquer creer un compte
-remplir le formulaire par
-nom complet: 
-email: teste@gmail.com
-mots de passe: testestes</t>
-  </si>
-  <si>
     <t>Test case</t>
   </si>
   <si>
@@ -487,6 +480,116 @@
   </si>
   <si>
     <t>revenir au login</t>
+  </si>
+  <si>
+    <t>chargement
+une notification d'erreur de duplication s'affiche</t>
+  </si>
+  <si>
+    <t>inscription avec message d'erreur</t>
+  </si>
+  <si>
+    <t>cliquer creer un compte
+remplir le formulaire par
+nom complet: testestes
+email: teste@gmail.com
+mots de passe: testestes
+cliquer s'inscrire</t>
+  </si>
+  <si>
+    <t>cliquer creer un compte
+remplir le formulaire par
+nom complet: Corontin Marque
+email: corontin@gmail.com
+mots de passe: testestes
+cliquer s'inscrire</t>
+  </si>
+  <si>
+    <t>chargement
+une notification de succes s'affiche</t>
+  </si>
+  <si>
+    <t>recuperation de mots de passe</t>
+  </si>
+  <si>
+    <t>cliquer sur recuperer mots de passe
+remplisser par zulmianah@gmail.com</t>
+  </si>
+  <si>
+    <t>un email de verification est envoye a zulmianah@gmail.com</t>
+  </si>
+  <si>
+    <t>profile</t>
+  </si>
+  <si>
+    <t>aller sur icon profile</t>
+  </si>
+  <si>
+    <t>chargement du profile</t>
+  </si>
+  <si>
+    <t>modifier mon profile</t>
+  </si>
+  <si>
+    <t>modifier le profile</t>
+  </si>
+  <si>
+    <t>chargement
+profile est modifie</t>
+  </si>
+  <si>
+    <t>modifier ma photo de profile</t>
+  </si>
+  <si>
+    <t>choisir par les photos locales ou prendre une nouvelle photo</t>
+  </si>
+  <si>
+    <t>chargement
+photo de profile est modifiee</t>
+  </si>
+  <si>
+    <t>points de ventes les plus proches</t>
+  </si>
+  <si>
+    <t>une carte s'affiche
+et les points de ventes les plus proches aussi</t>
+  </si>
+  <si>
+    <t>mon portefeuille</t>
+  </si>
+  <si>
+    <t>aller sur icon portefeuille</t>
+  </si>
+  <si>
+    <t>chargement de mon portefeuille et son affichage</t>
+  </si>
+  <si>
+    <t>acheter jetons</t>
+  </si>
+  <si>
+    <t>scanner</t>
+  </si>
+  <si>
+    <t>le solde devrait s'additionner</t>
+  </si>
+  <si>
+    <t>historique</t>
+  </si>
+  <si>
+    <t>aller dans historique</t>
+  </si>
+  <si>
+    <t>affichage des historique</t>
+  </si>
+  <si>
+    <t>notification</t>
+  </si>
+  <si>
+    <t>aller dans recherche
+glisser a droite pour suivre</t>
+  </si>
+  <si>
+    <t>notifier</t>
   </si>
 </sst>
 </file>
@@ -869,7 +972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -935,7 +1038,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>9</v>
@@ -1097,10 +1200,10 @@
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>41</v>
@@ -1111,10 +1214,10 @@
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>41</v>
@@ -1125,10 +1228,10 @@
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>41</v>
@@ -1139,13 +1242,13 @@
     </row>
     <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
@@ -1153,13 +1256,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>137</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
@@ -1173,10 +1276,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,50 +1363,199 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="D16" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D17" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="D18" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1330,18 +1582,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
         <v>59</v>
-      </c>
-      <c r="B1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1360,13 +1612,13 @@
     </row>
     <row r="4" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1374,10 +1626,10 @@
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -1385,10 +1637,10 @@
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -1396,13 +1648,13 @@
     </row>
     <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" t="s">
         <v>117</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>119</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1414,13 +1666,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>70</v>
-      </c>
-      <c r="C9" t="s">
-        <v>71</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -1428,10 +1680,10 @@
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -1439,10 +1691,10 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -1450,10 +1702,10 @@
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -1461,10 +1713,10 @@
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
@@ -1472,13 +1724,13 @@
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
@@ -1486,10 +1738,10 @@
     </row>
     <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
@@ -1497,10 +1749,10 @@
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
@@ -1508,13 +1760,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
@@ -1522,10 +1774,10 @@
     </row>
     <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
@@ -1533,13 +1785,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
@@ -1547,10 +1799,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="D23" t="s">
         <v>9</v>
@@ -1558,10 +1810,10 @@
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
@@ -1569,10 +1821,10 @@
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
@@ -1580,13 +1832,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="D27" t="s">
         <v>9</v>
@@ -1594,13 +1846,13 @@
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
@@ -1608,13 +1860,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" t="s">
         <v>106</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>107</v>
-      </c>
-      <c r="C32" t="s">
-        <v>108</v>
       </c>
       <c r="D32" t="s">
         <v>9</v>
@@ -1622,10 +1874,10 @@
     </row>
     <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
@@ -1633,10 +1885,10 @@
     </row>
     <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="D34" t="s">
         <v>9</v>
@@ -1644,13 +1896,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" t="s">
         <v>113</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>114</v>
-      </c>
-      <c r="C36" t="s">
-        <v>115</v>
       </c>
       <c r="D36" t="s">
         <v>9</v>

</xml_diff>